<commit_message>
Small update to MIFVAC_CRIANCA
</commit_message>
<xml_diff>
--- a/app/config/tables/MIFVAC_CRIANCA/forms/MIFVAC_CRIANCA/MIFVAC_CRIANCA.xlsx
+++ b/app/config/tables/MIFVAC_CRIANCA/forms/MIFVAC_CRIANCA/MIFVAC_CRIANCA.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4F05B3-717C-4AE8-B6DC-FC3116A36E74}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB84A61A-DF4F-40E0-9663-4DF7756E57FA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4599,7 +4599,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>